<commit_message>
add scope and functional requirements modifications& add questions in SIQ
</commit_message>
<xml_diff>
--- a/project_management/SIQ.xlsx
+++ b/project_management/SIQ.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -75,13 +75,25 @@
   </si>
   <si>
     <t>car datails(model,image,seller phone,seller name)?</t>
+  </si>
+  <si>
+    <t>Q_7</t>
+  </si>
+  <si>
+    <t>Car reservation by "reserve" button only?</t>
+  </si>
+  <si>
+    <t>Q_8</t>
+  </si>
+  <si>
+    <t>Car can be reserved by one person only?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -102,6 +114,21 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Aptos narrow"/>
+    </font>
+    <font>
+      <sz val="20.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="20.0"/>
+      <color theme="1"/>
+      <name val="Aptos narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -130,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -140,6 +167,19 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -450,12 +490,29 @@
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="C8" s="2"/>
+      <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="C9" s="2"/>
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
+      <c r="B10" s="9"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">

</xml_diff>